<commit_message>
- adjusted some plots and notebooks
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxik\Documents\Semester_6\Projektarbeit\github_repo\Steganography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAF03D8-027F-4438-9A1B-1A3F1E30A29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35118611-2D21-4022-8F8E-75CC6021B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="17952" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{F000BBA8-7058-4436-871D-188F12F109CE}"/>
+    <workbookView xWindow="45972" yWindow="17952" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F000BBA8-7058-4436-871D-188F12F109CE}"/>
   </bookViews>
   <sheets>
     <sheet name="cut" sheetId="5" r:id="rId1"/>
@@ -345,9 +345,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3483,6 +3484,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="176098112"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4515,6 +4517,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1458335712"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4604,350 +4607,6 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>recursion_new!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GAIN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>recursion_new!$A$3:$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>recursion_new!$F$3:$F$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EA28-4E99-9FEB-38E3D43F7C69}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="215932400"/>
-        <c:axId val="215932816"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="215932400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="215932816"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="215932816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="215932400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -5768,6 +5427,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="179600720"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5856,7 +5516,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -7015,6 +6675,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1230518320"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7103,7 +6764,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -8241,6 +7902,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="215919504"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -8329,7 +7991,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -9280,6 +8942,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="172407984"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -9608,46 +9271,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -12164,509 +11787,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13243,42 +12363,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>337820</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>128270</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>90170</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{643E3AD9-287B-4DBE-8ED2-E8DEF1363F3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13551,13 +12635,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6E8BDA29-66DF-4473-B82A-19B2AD4A93C5}" name="metrics__4" displayName="metrics__4" ref="A1:G102" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G102" xr:uid="{6E8BDA29-66DF-4473-B82A-19B2AD4A93C5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9077AC47-1718-4181-9826-5A7EAFFEE5D6}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{17B3C678-0F08-4AF7-92CD-039F7CDF4345}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{5AA5590A-C3BF-426F-8410-090D30744574}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{B0F62079-EF12-4B0C-8A64-C02395F79E43}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{AB62C5C2-0601-40F7-B21D-F7D6045117F3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{B25A813D-FA18-477B-BB51-E4258E1C2205}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{0436947C-1852-421A-89B4-7FE4110C7740}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{9077AC47-1718-4181-9826-5A7EAFFEE5D6}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{17B3C678-0F08-4AF7-92CD-039F7CDF4345}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{5AA5590A-C3BF-426F-8410-090D30744574}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{B0F62079-EF12-4B0C-8A64-C02395F79E43}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{AB62C5C2-0601-40F7-B21D-F7D6045117F3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{B25A813D-FA18-477B-BB51-E4258E1C2205}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{0436947C-1852-421A-89B4-7FE4110C7740}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13567,13 +12651,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B8B90ACE-8D0D-4CB5-A690-28236A3318EC}" name="metrics__5" displayName="metrics__5" ref="A1:G12" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G12" xr:uid="{B8B90ACE-8D0D-4CB5-A690-28236A3318EC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2B04757E-F3F7-4628-A151-81DB95F30BF8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{CB49E5D2-8CF3-4E90-B1EF-C23DD8C47347}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{D5702EDA-B620-4B1E-A967-B14423063460}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4B3ACF0C-0089-49AA-B810-87B9EA70502E}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{C3812B9C-A286-4068-A2BB-6FA58C833A2C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{CF3B8385-FAA8-4447-B487-B7FDE4E2B417}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{CAAB8C0D-A266-4BAF-A801-98243FAD9709}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{2B04757E-F3F7-4628-A151-81DB95F30BF8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{CB49E5D2-8CF3-4E90-B1EF-C23DD8C47347}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{D5702EDA-B620-4B1E-A967-B14423063460}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{4B3ACF0C-0089-49AA-B810-87B9EA70502E}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{C3812B9C-A286-4068-A2BB-6FA58C833A2C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{CF3B8385-FAA8-4447-B487-B7FDE4E2B417}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{CAAB8C0D-A266-4BAF-A801-98243FAD9709}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13599,13 +12683,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A529BC9C-D4D1-417E-8A25-170F77F6DBC0}" name="metrics__6" displayName="metrics__6" ref="A1:G19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G19" xr:uid="{A529BC9C-D4D1-417E-8A25-170F77F6DBC0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B7701B3B-8052-4476-82A9-281BBA8A38D7}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B055FCD4-A472-412A-BEF5-41A44DC7AC8A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E3E89493-BFAB-4EDB-9459-09A92657B79F}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{5EAF5281-9E41-4086-B537-390209942AD3}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D3B6542B-7CDF-4EA8-BB4C-79BD991F3322}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{1817B654-5DBA-42DE-B004-F2BF61C09F80}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B9D3E683-45C5-49CF-B210-9125E259AEE9}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B7701B3B-8052-4476-82A9-281BBA8A38D7}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{B055FCD4-A472-412A-BEF5-41A44DC7AC8A}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{E3E89493-BFAB-4EDB-9459-09A92657B79F}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{5EAF5281-9E41-4086-B537-390209942AD3}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{D3B6542B-7CDF-4EA8-BB4C-79BD991F3322}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{1817B654-5DBA-42DE-B004-F2BF61C09F80}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B9D3E683-45C5-49CF-B210-9125E259AEE9}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13615,13 +12699,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2650B976-17B4-4813-A87E-8871A2849384}" name="metrics__2" displayName="metrics__2" ref="A1:G18" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G18" xr:uid="{2650B976-17B4-4813-A87E-8871A2849384}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C9D69236-0FEF-4CAB-A0D9-C7B8AAC55FD1}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{A77E532E-53F9-4443-80BF-8A6E91B7DEC7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{C6B4ED39-FE33-48CD-B028-86C0784C813D}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{92A41CAA-E835-4034-A53B-EF972E17AABF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{2ED8CF9F-F89D-456A-86E0-B5609989EB34}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{A9677C4E-FDCD-4557-B4C3-4A82FE24A4CD}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{B22A7587-8C05-40A8-99BB-1957EC4F4E00}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{C9D69236-0FEF-4CAB-A0D9-C7B8AAC55FD1}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{A77E532E-53F9-4443-80BF-8A6E91B7DEC7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C6B4ED39-FE33-48CD-B028-86C0784C813D}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{92A41CAA-E835-4034-A53B-EF972E17AABF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2ED8CF9F-F89D-456A-86E0-B5609989EB34}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{A9677C4E-FDCD-4557-B4C3-4A82FE24A4CD}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{B22A7587-8C05-40A8-99BB-1957EC4F4E00}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13631,13 +12715,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86A77D59-F0E9-4A6C-836A-C6FF5D6A0C85}" name="metrics" displayName="metrics" ref="A1:G12" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G12" xr:uid="{86A77D59-F0E9-4A6C-836A-C6FF5D6A0C85}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7347599E-45CF-4A73-B453-F2EEB7FC765D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{7D244F76-2AF5-44F0-AED9-687B2C36C3B7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{403CB007-F929-4CCE-AE29-924EDD5364DC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{DA6EDDB4-1F5C-4583-8AFA-9B83FA3F5B63}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{931C44E9-038D-4461-9039-94516A2BBF2C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{F974102B-37AE-4D07-83D8-6A4778D7E123}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{67703FD5-96EB-4CC5-BA92-C5B29A253F68}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{7347599E-45CF-4A73-B453-F2EEB7FC765D}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7D244F76-2AF5-44F0-AED9-687B2C36C3B7}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{403CB007-F929-4CCE-AE29-924EDD5364DC}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DA6EDDB4-1F5C-4583-8AFA-9B83FA3F5B63}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{931C44E9-038D-4461-9039-94516A2BBF2C}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F974102B-37AE-4D07-83D8-6A4778D7E123}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{67703FD5-96EB-4CC5-BA92-C5B29A253F68}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16320,8 +15404,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -16395,7 +15479,7 @@
       <c r="E3" s="1">
         <v>0.4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="1">
@@ -16418,7 +15502,7 @@
       <c r="E4" s="1">
         <v>0.4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="1">
@@ -16441,7 +15525,7 @@
       <c r="E5" s="1">
         <v>0.4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G5" s="1">
@@ -16464,7 +15548,7 @@
       <c r="E6" s="1">
         <v>0.4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="1">
@@ -16487,7 +15571,7 @@
       <c r="E7" s="1">
         <v>0.4</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="1">
@@ -16510,7 +15594,7 @@
       <c r="E8" s="1">
         <v>0.4</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G8" s="1">
@@ -16533,7 +15617,7 @@
       <c r="E9" s="1">
         <v>0.4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="G9" s="1">
@@ -16556,7 +15640,7 @@
       <c r="E10" s="1">
         <v>0.4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G10" s="1">
@@ -16579,7 +15663,7 @@
       <c r="E11" s="1">
         <v>0.4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>61</v>
       </c>
       <c r="G11" s="1">
@@ -16602,7 +15686,7 @@
       <c r="E12" s="1">
         <v>0.4</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>64</v>
       </c>
       <c r="G12" s="1">
@@ -16611,9 +15695,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -17838,7 +16923,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to README and requirements.yml
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxik\Documents\Semester_6\Projektarbeit\github_repo\Steganography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35118611-2D21-4022-8F8E-75CC6021B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE98EF4C-9303-4BDE-949F-FE7D9A06A0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="17952" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F000BBA8-7058-4436-871D-188F12F109CE}"/>
+    <workbookView xWindow="46692" yWindow="12672" windowWidth="22536" windowHeight="13176" xr2:uid="{F000BBA8-7058-4436-871D-188F12F109CE}"/>
   </bookViews>
   <sheets>
     <sheet name="cut" sheetId="5" r:id="rId1"/>
@@ -3440,7 +3440,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Werte cut in 1% Schritten, 1. Wert:</a:t>
+                  <a:t>Values</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> depicted in 1% steps;</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t> 1. Value:</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" baseline="0"/>
@@ -3608,11 +3616,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>REKURSION</a:t>
+              <a:t>gain optimization</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> TEST (mandril)</a:t>
+              <a:t> (mandril)</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -6635,7 +6643,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> (Anzahl utf-8 Zeichen)</a:t>
+                  <a:t> (utf-8 symbols)</a:t>
                 </a:r>
                 <a:endParaRPr lang="de-DE"/>
               </a:p>
@@ -12417,15 +12425,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>154940</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>142240</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>375920</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>48260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13029,8 +13037,8 @@
   </sheetPr>
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -15404,8 +15412,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -15711,7 +15719,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -16014,8 +16022,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -16923,8 +16931,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>